<commit_message>
update template to match order of documentation
</commit_message>
<xml_diff>
--- a/metadata_templates/HP_manuscript_metadata_template.xlsx
+++ b/metadata_templates/HP_manuscript_metadata_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/mrbst20_pitt_edu/Documents/ULS_Work/DigitalCollections/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelbolam/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{2759F48C-FB9B-D34B-BFD0-779D55278F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78065AEB-E3ED-194B-8EEF-F79A50292EBB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D52D2BB-D727-AC40-B376-C01811DB6281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{5BC5E1C4-B012-954E-9572-934211487BD1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{5BC5E1C4-B012-954E-9572-934211487BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>title</t>
   </si>
@@ -48,9 +48,6 @@
     <t>normalized_date_qualifier</t>
   </si>
   <si>
-    <t>abstract</t>
-  </si>
-  <si>
     <t>subject</t>
   </si>
   <si>
@@ -91,6 +88,30 @@
   </si>
   <si>
     <t>source_citation</t>
+  </si>
+  <si>
+    <t>subject_location</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>rights_holder</t>
+  </si>
+  <si>
+    <t>depositor</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>contributor</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>source_id</t>
   </si>
 </sst>
 </file>
@@ -446,41 +467,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF565F6-0AA2-6045-BDB2-0D376AF771A0}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" customWidth="1"/>
+    <col min="13" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="16" max="16" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" customWidth="1"/>
+    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
@@ -489,31 +535,49 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -522,6 +586,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A8D8FC47DE7C204786C404ECD83547D9" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3cf0c2705b82825f0346af526cda3b2b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7f1a2e88-5503-46a0-aef8-44b94e11b624" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="749d39a5ac9e1b1b5c892e0bcc9b56c2" ns2:_="">
     <xsd:import namespace="7f1a2e88-5503-46a0-aef8-44b94e11b624"/>
@@ -667,12 +737,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -683,6 +747,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAE04D26-0F78-42B0-8B91-19CD11EAF985}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7f1a2e88-5503-46a0-aef8-44b94e11b624"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{542B4DC3-755E-4A14-8750-25BF73587E37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -700,22 +780,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAE04D26-0F78-42B0-8B91-19CD11EAF985}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7f1a2e88-5503-46a0-aef8-44b94e11b624"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43179E9D-8E53-46CD-8BA7-E72C1E77F56D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added language to manuscript template
</commit_message>
<xml_diff>
--- a/metadata_templates/HP_manuscript_metadata_template.xlsx
+++ b/metadata_templates/HP_manuscript_metadata_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelbolam/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelbolam/Documents/GitHub/MAD_Islandora_Metadata/islandora_metadata/metadata_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D52D2BB-D727-AC40-B376-C01811DB6281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492F8D20-51D4-8C49-B919-28B9FA9D80F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{5BC5E1C4-B012-954E-9572-934211487BD1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{5BC5E1C4-B012-954E-9572-934211487BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>title</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>source_id</t>
+  </si>
+  <si>
+    <t>language</t>
   </si>
 </sst>
 </file>
@@ -467,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF565F6-0AA2-6045-BDB2-0D376AF771A0}">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,21 +489,23 @@
     <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" customWidth="1"/>
-    <col min="13" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" customWidth="1"/>
-    <col min="16" max="16" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18" customWidth="1"/>
-    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
+    <col min="17" max="17" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" customWidth="1"/>
+    <col min="21" max="21" width="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,42 +546,45 @@
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -592,6 +600,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A8D8FC47DE7C204786C404ECD83547D9" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3cf0c2705b82825f0346af526cda3b2b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7f1a2e88-5503-46a0-aef8-44b94e11b624" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="749d39a5ac9e1b1b5c892e0bcc9b56c2" ns2:_="">
     <xsd:import namespace="7f1a2e88-5503-46a0-aef8-44b94e11b624"/>
@@ -737,15 +754,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAE04D26-0F78-42B0-8B91-19CD11EAF985}">
   <ds:schemaRefs>
@@ -763,6 +771,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43179E9D-8E53-46CD-8BA7-E72C1E77F56D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{542B4DC3-755E-4A14-8750-25BF73587E37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -778,12 +794,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43179E9D-8E53-46CD-8BA7-E72C1E77F56D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>